<commit_message>
Updated with Spring boot End 2 End Low code integration testing - Self certification
</commit_message>
<xml_diff>
--- a/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
+++ b/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24020"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23D094D5-D1DF-4D4E-B35C-7D708917C4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8000DF7-4E0B-4FAE-A1C6-A623713274C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,10 +92,9 @@
     "resource": "pets",
     "url": "/pets/findByTags",
     "type": "Params",
-    "rule": "[{\"tags\":\"spring-grey
-\"}]",
+    "rule": "[{\"tags\":\"spring-grey\"}]",
     "operationId": "findPetsByTags",
-    "output": "\"{\n  \"category\": {\n    \"id\": 200,\n    \"name\": \"Bulldog\"\n  },\n  \"id\": 201,\n  \"name\": \"Butch\",\n  \"photoUrls\": [\n    \"string\"\n  ],\n  \"status\": \"available\",\n  \"tags\": [\n    {\n      \"id\": 201,\n      \"name\": \"&lt;tags&gt;\"\n    }\n  ]\n}",
+    "output": "{\n  \"category\": {\n    \"id\": 200,\n    \"name\": \"Bulldog\"\n  },\n  \"id\": 201,\n  \"name\": \"Butch\",\n  \"photoUrls\": [\n    \"string\"\n  ],\n  \"status\": \"available\",\n  \"tags\": [\n    {\n      \"id\": 201,\n      \"name\": \"&lt;tags&gt;\"\n    }\n  ]\n}",
     "httpStatusCode": "200",
     "method": "GET",
     "availableParams": [
@@ -144,7 +143,7 @@
   </si>
   <si>
     <t>id,name,category/id:name,photoUrls,status,tags/id:name
-201,Butch,200:Bulldog,string\|,available,201,grey\|</t>
+i~201,Butch,i~200:Bulldog,string\|,available,i~201:spring-grey\|</t>
   </si>
   <si>
     <t>AddMockDataForPOST</t>
@@ -158,8 +157,8 @@
     "url": "/pets",
     "type": "Response",
     "operationId": "addPet",
-    "input": "{\n  \"category\": {\n    \"id\": 100,\n    \"name\": \"string\" \n  },\n  \"id\": 100,\n  \"name\": \"doggie-1\"",\n  \"photoUrls\": [\n    \"string\" \n  ],\n  \"status\": \"available\"",\n  \"tags\": [\n    {\n      \"id\": 0,\n      \"name\": \"string\" \n    }\n  ]\n}\"",
-    "output": "\"{\n  \"category\": {\n    \"id\": 100,\n    \"name\": \"string\" \n  },\n  \"id\": 100,\n  \"name\": \"doggie\"",\n  \"photoUrls\": [\n    \"string\" \n  ],\n  \"status\": \"available\"",\n  \"tags\": [\n    {\n      \"id\": 0,\n      \"name\": \"string\" \n    }\n  ]\n}\"",
+    "input": "{\n  \"category\": {\n    \"id\": 100,\n    \"name\": \"string\" \n  },\n  \"id\": 100,\n  \"name\": \"doggie-1\",\n  \"photoUrls\": [\n    \"string\" \n  ],\n  \"status\": \"available\",\n  \"tags\": [\n    {\n      \"id\": 0,\n      \"name\": \"string\" \n    }\n  ]\n}",
+    "output": "{\n  \"category\": {\n    \"id\": 100,\n    \"name\": \"string\" \n  },\n  \"id\": 100,\n  \"name\": \"doggie\",\n  \"photoUrls\": [\n    \"string\" \n  ],\n  \"status\": \"available\",\n  \"tags\": [\n    {\n      \"id\": 0,\n      \"name\": \"string\" \n    }\n  ]\n}",
     "httpStatusCode": "201",
     "method": "POST"
 }</t>
@@ -576,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -711,7 +710,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="280.5">
+    <row r="5" spans="1:11" ht="267.75">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Updated with new release changes with AsyncAPI mocking
</commit_message>
<xml_diff>
--- a/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
+++ b/samples/virtualan-spring-boot/src/test/resources/virtualan_bdd_testcase_run_manager_1.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8000DF7-4E0B-4FAE-A1C6-A623713274C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\July13\virtualan\samples\virtualan-spring-boot\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE656CD3-2AE4-42FE-8E48-B7A2A1301EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API-Testing" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -71,9 +76,6 @@
   </si>
   <si>
     <t>application/json</t>
-  </si>
-  <si>
-    <t>code=MOCK_DATA_NOT_SET</t>
   </si>
   <si>
     <t>GET</t>
@@ -575,19 +577,19 @@
   </sheetPr>
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="176.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="176.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.71875" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="8" width="22.140625" customWidth="1"/>
+    <col min="7" max="8" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -639,57 +641,55 @@
         <v>14</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="255">
+    <row r="3" spans="1:11" ht="332.7">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" s="2">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="150">
+    <row r="4" spans="1:11" ht="270">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -697,74 +697,74 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="267.75">
+    <row r="5" spans="1:11" ht="295.8">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" s="2">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="126">
+    <row r="6" spans="1:11" ht="280.8">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" s="1">
         <v>201</v>

</xml_diff>